<commit_message>
fix CAN spreadsheet, fix kv calcs
</commit_message>
<xml_diff>
--- a/CANBusConfig.xlsx
+++ b/CANBusConfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davor\SynologyDrive\SynologyDrive\University\Capstone\MiniFOCer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D399DF-879D-4084-8B8A-B3184ACA87E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50C9A82-9524-4914-8F2B-C35C06A0790E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{057639FE-E767-4E97-94AE-602186CEC3E6}"/>
   </bookViews>
@@ -71,12 +71,6 @@
     <t>0x201708</t>
   </si>
   <si>
-    <t>Motor 1 current * 0.01 (int16)</t>
-  </si>
-  <si>
-    <t>Motor 2 current * 0.01 (int16)</t>
-  </si>
-  <si>
     <t>Direction</t>
   </si>
   <si>
@@ -107,30 +101,12 @@
     <t>0x801402</t>
   </si>
   <si>
-    <t>Bus voltage * 0.01 (int16)</t>
-  </si>
-  <si>
-    <t>Gate driver voltage * 0.01 (int16)</t>
-  </si>
-  <si>
     <t>Status 3</t>
   </si>
   <si>
     <t>0x801502</t>
   </si>
   <si>
-    <t>Motor 1 quadrature command * 0.001 (int16)</t>
-  </si>
-  <si>
-    <t>Motor 2 quadrature command * 0.001 (int16)</t>
-  </si>
-  <si>
-    <t>Motor 1 direct command * 0.001 (int16)</t>
-  </si>
-  <si>
-    <t>Motor 2 direct command * 0.001 (int16)</t>
-  </si>
-  <si>
     <t>Config</t>
   </si>
   <si>
@@ -143,12 +119,6 @@
     <t>Max abs current * 0.2 (uint8)</t>
   </si>
   <si>
-    <t>UVLO hyst * 0.01 (uint8)</t>
-  </si>
-  <si>
-    <t>UVLO voltage * 0.1 (uint8)</t>
-  </si>
-  <si>
     <t>Errors: |x|x|x|x|x|OC1|OC2|UV|</t>
   </si>
   <si>
@@ -188,12 +158,6 @@
     <t>0x801602</t>
   </si>
   <si>
-    <t>M1 meas current * 0.1 (uint8)</t>
-  </si>
-  <si>
-    <t>M2 meas current * 0.1 (uint8)</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -213,6 +177,42 @@
   </si>
   <si>
     <t>M2 offset (uint16)</t>
+  </si>
+  <si>
+    <t>Motor 1 current * 100 (int16)</t>
+  </si>
+  <si>
+    <t>Motor 2 current * 100 (int16)</t>
+  </si>
+  <si>
+    <t>Bus voltage * 100 (int16)</t>
+  </si>
+  <si>
+    <t>Gate driver voltage * 100 (int16)</t>
+  </si>
+  <si>
+    <t>Motor 1 quadrature command * 1000 (int16)</t>
+  </si>
+  <si>
+    <t>Motor 2 quadrature command * 1000 (int16)</t>
+  </si>
+  <si>
+    <t>Motor 1 direct command * 1000 (int16)</t>
+  </si>
+  <si>
+    <t>Motor 2 direct command * 1000 (int16)</t>
+  </si>
+  <si>
+    <t>UVLO voltage * 10 (uint8)</t>
+  </si>
+  <si>
+    <t>UVLO hyst * 100 (uint8)</t>
+  </si>
+  <si>
+    <t>M1 meas current * 10 (uint8)</t>
+  </si>
+  <si>
+    <t>M2 meas current * 10 (uint8)</t>
   </si>
 </sst>
 </file>
@@ -332,13 +332,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,7 +678,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -723,29 +723,29 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="D2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="9"/>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -753,51 +753,51 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -805,52 +805,52 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -859,98 +859,106 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8" t="s">
+      <c r="K8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="L8" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="8"/>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="D9:E9"/>
@@ -959,14 +967,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>